<commit_message>
fix: update selectbox options to include unique and sorted expense elements
</commit_message>
<xml_diff>
--- a/dados/base_insumos.xlsx
+++ b/dados/base_insumos.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmagi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D862FA0-860B-45CE-AFC7-6DD3BA93B8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168D7975-382E-400E-A034-36EF1480597C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2A84FFDB-6AAA-49C1-8EF7-A10CB5CC52A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{2A84FFDB-6AAA-49C1-8EF7-A10CB5CC52A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$256</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="420">
   <si>
     <t>Elemento de Despesa</t>
   </si>
@@ -887,9 +890,6 @@
     <t>Água Mineral - Garrafão de 20L</t>
   </si>
   <si>
-    <t>Garrafões de água mineral de 20 litros e copos descartáveis tipo para uso em bebedouro. No preço unitário do garrafão devem estar agregados todos os custos acima descritos.</t>
-  </si>
-  <si>
     <t>Água Mineral Garrafas - 300 ml</t>
   </si>
   <si>
@@ -911,9 +911,6 @@
     <t>Brunch</t>
   </si>
   <si>
-    <t>Sugestão a) Bebidas: café, chá, suco de fruta (02 tipos), refrigerante (2 tipos); b) Comidas: frutas frescas fatiadas (melão, melancia, manga, kivi, etc), queijos variados (massadã, provólone, parmesão, etc), presunto cru, salmão defumado, sanduchinhos de peru defumado e de tomate seco com mussarela de búfala, strudel de palmito com mussarela, salada verde com bacon, torradas, lascas de parmesão e figo fresco, salada de alface americana com berinjela, azeitona preta e passas, mousse de ricota com maracujá e molho de mostarda a parte, cesta de pães, massa e tortas salgadas: penne com molho de espinafre, espaguete ao sugo, raviole de queijo com molho de gorgonzola, torta de frango com catu­piry, torta de carne seca com abóbora, torta de palmito, etc. Sobremesa: bolo de casamento (pão de ló recheado com creme e morangos fresco), tor­ti­nhas individuais de frutas variadas, bem casados, doce de leite, mousses variadas. SEMPRE CONSIDERAR OPÇÕES VEGANAS E ZERO AÇÚCAR. PARA EVENTOS COM MAIS DE 1 (UM) DIA DE DURAÇÃO, VARIAR OS CARDÁPIOS DIÁRIOS. INCLUSO MÃO DE OBRA E UTENSÍLIOS.</t>
-  </si>
-  <si>
     <t>Coffee Break (Tipo 1)</t>
   </si>
   <si>
@@ -929,9 +926,6 @@
     <t>Garrafa de Café</t>
   </si>
   <si>
-    <t>Garrafias térmicas com café com capacidade de 1 litro com copos descartáveis, açúcar e adoçante em sachês pelo período dos eventos;</t>
-  </si>
-  <si>
     <t>Marmitex</t>
   </si>
   <si>
@@ -941,18 +935,9 @@
     <t>Petit Four</t>
   </si>
   <si>
-    <t>Mínimo 8 (oito) opções. Sugestão: Biscoitos finos de polvilho, amanteigados, nata, pequenos recheados com geleias, casadinho com goiabada, leite condensado, gravatinha, bambolê, coco flocos, mentirinha, sequilho, cocadinha, bolos diversos, entre outros. SEMPRE CONSIDERAR OPÇÕES ZERO AÇÚCAR. INCLUSO MÃO DE OBRA E UTENSÍLIOS.</t>
-  </si>
-  <si>
     <t>Garrafões de água mineral de 20 litros e copos descartáveis tipo para uso em bebedouro. No preço unitário do garrafão devem estar agregados todos os custos acima descritos;</t>
   </si>
   <si>
-    <t>Sugestão: a) Entrada: pão sírio ou pãezinhos integrais com; b) Salada: 2 opções - vegetais folhosos, vegetais crus e cozidos, frutas da estação – 02 (duas) opções; c) Guarnições: 3 opções - arroz branco ou com vegetais (brócolis, cenoura, vagem, etc), feijão simples (sem farinhas ou carnes tipos charque, calabresa, bacon, etc), batata assada, legumes sauté, legumes cozidos; d) Pratos principais: 2 opções - bife acebolado grelhado, frango com legumes, carne assada ou frango grelhado ou assado; e) Sobremessira: 2 opções - salada de frutas, gelatina, frutas; f) Bebidas: 2 opções de cada - refrigerante, suco de fruta ou água com ou sem gás de 300ml. SEMPRE CONSIDERAR OPÇÕES VEGANAIS E ZERO AÇÚCAR. PARA EVENTOS COM MAIS DE 1 (UM) DIA DE DURAÇÃO, VARIAR OS CARDAPIOS DIÁRIOS. INCLUSO MÃO DE OBRA E UTENSÍLIOS.</t>
-  </si>
-  <si>
-    <t>Sugestão: a) Entrada: pão sírio ou pãezinhos integrais com; b) Salada: 2 opções - vegetais folhosos, vegetais crus e cozidos, frutas da estação – 02 (duas) opções; c) Guarnições: 3 opções - arroz branco ou com vegetais (brócolis, cenoura, vagem, etc) b) Pratos principais: 2 opções - medalhão de filé ao molho madeira, escalopinho ao molho mostarda, estrogonofe de filé, supremo de frango, peito de peru; d) Sobremesas: 2 opções - sorvete com cobertura, salada de frutas com chantaje, pudim de leite, pavê, torta de frutas; e) Bebidas: 4 opções - refrigerante, suco de fruta, água com ou sem gás, ou coquetel de frutas sem álcool 300ml. SEMPRE CONSIDERAR OPÇÕES VEGANAS E ZERO AÇÚCAR. PARA EVENTOS COM MAIS DE 1 (UM) DIA DE DURAÇÃO, VARIAR OS CARDÁPIOS DIÁRIOS. INCLUSO MÃO DE OBRA E UTENSÍLIOS.</t>
-  </si>
-  <si>
     <t>Sugestão: a) Bebidas: café, chá, suco de fruta (02 tipos), refrigerante (2 tipos); b) Comidas: frutas frescas fatiadas (melão, melancia, manga, kivi, etc), queijos variados (mascada, provolone, parmesão, etc), presunto cru, salmão defumado, sanduichinhos de pert defumado e de tomate seco com mussarela de búfala, strudel de palmito com mussarela, salada verde com bacon, torradas, lascas de parmesão e figo fresco, salada de alface americana com berinjela, azeitona preta e passas, mousse de ricota com maracujá e molho de mostarda a parte, cesta de pães, massa e tortas salgadas: penne com molho de espinafre, espaguete ao sugo, raviole de queijo com molho de gorgonzola, torta de frango com catupiry, torta de carne seca com abóbora, torta de palmito, etc. Sobremesa: bolo de casamento (pão de ló recheado com creme e morangos fresco), tortinhas individuais de frutas variadas, bem casados, doce de leite, mousses variadas. SEMPRE CONSIDERAR OPÇÕES VEGANAS E ZERO AÇÚCAR. INCLUSO MÃO DE OBRA E UTENSÍLIOS</t>
   </si>
   <si>
@@ -965,9 +950,6 @@
     <t>Coffee Break ou wecleome coffe (Tipo 2)</t>
   </si>
   <si>
-    <t>Sugestão: a) Entrada: pão sírio ou pãezinhos integrais com; b) Salada: 2 opções - vegetais folhosos, vegetais crus e cozidos, frutas da estação – 02 (duas) opções; c) Guarnições: 3 opções - arroz branco ou com vegetais (brócolis, cenoura, vagem, etc) Comidas: até 10 opções - pão de queijo, pão da vovó, pão húngaro, pão de batata com presunto e queijo, rosea calabresa, broa de milho com gergelim, enroladinho de queijo com orégano e tomate, enroladinho queijo e coco, religiosa de frango, mini sonhos, mini croissants de queijo, mini croissants com ervas finas, mini croissants com gergelim e catupity, mini sanduíche natural, mini bom-bocado, mini pudim, mini pizzas, mini rabanadas, empadinha de frango, pastel milho de forno, biscoito de queijo palito, biscoitos amanteigados, frios variados fatiados, queijos variados fatiados, rosquinhas de leite condensado, barquetes de legumes, bolos tipo inglês, formigueiro, laranja, chocolate; queijadinha, petit fours doces e salgados, frutas variadas fatiadas, mini canapé. Frutas da estação laminadas ou salda de frutas. SEMPRE CONSIDERAR OPÇÕES VEGANAS E ZERO AÇÚCAR. INCLUSO MÃO DE OBRA E UTENSÍLIOS.</t>
-  </si>
-  <si>
     <t>Garrafas térmicas com café com capacidade de 1 litro com copos descartáveis, açúcar e adoçante em sachês pelo período dos eventos;</t>
   </si>
   <si>
@@ -1314,6 +1296,9 @@
   </si>
   <si>
     <t>Veículo motorizado equipado com som em potência permitida por lei local, para divulgação sonora de anúncios e informativos de utilidade pública. Com motorista e equipamento.</t>
+  </si>
+  <si>
+    <t>INCLUSO MÃO DE OBRA E UTENSÍLIOS. Sugestão: a) Entrada: pão sírio ou pãezinhos integrais com; b) Salada: 2 opções - vegetais folhosos, vegetais crus e cozidos, frutas da estação – 02 (duas) opções; c) Guarnições: 3 opções - arroz branco ou com vegetais (brócolis, cenoura, vagem, etc) Comidas: até 10 opções - pão de queijo, pão da vovó, pão húngaro, pão de batata com presunto e queijo, rosea calabresa, broa de milho com gergelim, enroladinho de queijo com orégano e tomate, enroladinho queijo e coco, religiosa de frango, mini sonhos, mini croissants de queijo, mini croissants com ervas finas, mini croissants com gergelim e catupity, mini sanduíche natural, mini bom-bocado, mini pudim, mini pizzas, mini rabanadas, empadinha de frango, pastel milho de forno, biscoito de queijo palito, biscoitos amanteigados, frios variados fatiados, queijos variados fatiados, rosquinhas de leite condensado, barquetes de legumes, bolos tipo inglês, formigueiro, laranja, chocolate; queijadinha, petit fours doces e salgados, frutas variadas fatiadas, mini canapé. Frutas da estação laminadas ou salda de frutas. SEMPRE CONSIDERAR OPÇÕES VEGANAS E ZERO AÇÚCAR.</t>
   </si>
 </sst>
 </file>
@@ -1321,10 +1306,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1335,6 +1320,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1360,11 +1358,20 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moeda 2" xfId="2" xr:uid="{C633EE3A-D3DC-4E25-8140-CB9635B9DE92}"/>
@@ -1701,18 +1708,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8A3085-2C8F-4430-ACE1-8267A727A491}">
-  <dimension ref="A1:E263"/>
+  <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="38.54296875" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
+    <col min="3" max="3" width="78" customWidth="1"/>
+    <col min="4" max="5" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1729,7 +1739,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>161</v>
       </c>
@@ -1743,7 +1753,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -1757,7 +1767,7 @@
         <v>4725</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -1771,7 +1781,7 @@
         <v>3360</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -1785,7 +1795,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -1799,7 +1809,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1813,7 +1823,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>164</v>
       </c>
@@ -1841,7 +1851,7 @@
         <v>6090</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -1855,7 +1865,7 @@
         <v>8295</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -1869,7 +1879,7 @@
         <v>3045</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>164</v>
       </c>
@@ -1883,7 +1893,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>164</v>
       </c>
@@ -1897,7 +1907,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>164</v>
       </c>
@@ -1911,7 +1921,7 @@
         <v>682.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -1939,7 +1949,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>164</v>
       </c>
@@ -1953,7 +1963,7 @@
         <v>3097.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>164</v>
       </c>
@@ -1967,7 +1977,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>164</v>
       </c>
@@ -1981,7 +1991,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>164</v>
       </c>
@@ -1995,7 +2005,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>164</v>
       </c>
@@ -2009,7 +2019,7 @@
         <v>4095</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>164</v>
       </c>
@@ -2023,7 +2033,7 @@
         <v>4725</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -2037,7 +2047,7 @@
         <v>787.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>164</v>
       </c>
@@ -2051,7 +2061,7 @@
         <v>3675</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>164</v>
       </c>
@@ -2065,7 +2075,7 @@
         <v>4305</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>164</v>
       </c>
@@ -2079,7 +2089,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>164</v>
       </c>
@@ -2093,7 +2103,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>164</v>
       </c>
@@ -2107,7 +2117,7 @@
         <v>3811.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>177</v>
       </c>
@@ -2121,7 +2131,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>177</v>
       </c>
@@ -2135,7 +2145,7 @@
         <v>3885</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>177</v>
       </c>
@@ -2149,7 +2159,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>177</v>
       </c>
@@ -2163,7 +2173,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>177</v>
       </c>
@@ -2177,7 +2187,7 @@
         <v>3675</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>177</v>
       </c>
@@ -2191,7 +2201,7 @@
         <v>4830</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -2205,7 +2215,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>177</v>
       </c>
@@ -2219,7 +2229,7 @@
         <v>33490</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>177</v>
       </c>
@@ -2233,7 +2243,7 @@
         <v>5250</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>177</v>
       </c>
@@ -2247,7 +2257,7 @@
         <v>1501.5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>177</v>
       </c>
@@ -2261,7 +2271,7 @@
         <v>724.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>180</v>
       </c>
@@ -2275,7 +2285,7 @@
         <v>793800</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>180</v>
       </c>
@@ -2289,7 +2299,7 @@
         <v>68985</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>180</v>
       </c>
@@ -2303,7 +2313,7 @@
         <v>91035</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>180</v>
       </c>
@@ -2317,7 +2327,7 @@
         <v>32602</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>180</v>
       </c>
@@ -2331,7 +2341,7 @@
         <v>37485</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>180</v>
       </c>
@@ -2345,7 +2355,7 @@
         <v>47460</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>180</v>
       </c>
@@ -2359,7 +2369,7 @@
         <v>59535</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>180</v>
       </c>
@@ -2373,7 +2383,7 @@
         <v>42630</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>180</v>
       </c>
@@ -2387,7 +2397,7 @@
         <v>38850</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>180</v>
       </c>
@@ -2401,7 +2411,7 @@
         <v>89250</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>180</v>
       </c>
@@ -2415,7 +2425,7 @@
         <v>20790</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>180</v>
       </c>
@@ -2429,7 +2439,7 @@
         <v>18585</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>180</v>
       </c>
@@ -2443,7 +2453,7 @@
         <v>89250</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>180</v>
       </c>
@@ -2457,7 +2467,7 @@
         <v>20790</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>180</v>
       </c>
@@ -2471,7 +2481,7 @@
         <v>18795</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>180</v>
       </c>
@@ -2485,7 +2495,7 @@
         <v>89250</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>180</v>
       </c>
@@ -2499,7 +2509,7 @@
         <v>26250</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>180</v>
       </c>
@@ -2513,7 +2523,7 @@
         <v>20790</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>180</v>
       </c>
@@ -2527,7 +2537,7 @@
         <v>18795</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>180</v>
       </c>
@@ -2541,7 +2551,7 @@
         <v>136500</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>180</v>
       </c>
@@ -2555,7 +2565,7 @@
         <v>28875</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>180</v>
       </c>
@@ -2569,7 +2579,7 @@
         <v>107100</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>180</v>
       </c>
@@ -2583,7 +2593,7 @@
         <v>136500</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>180</v>
       </c>
@@ -2597,7 +2607,7 @@
         <v>29610</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>180</v>
       </c>
@@ -2611,7 +2621,7 @@
         <v>26775</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>180</v>
       </c>
@@ -2625,7 +2635,7 @@
         <v>26145</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>180</v>
       </c>
@@ -2639,7 +2649,7 @@
         <v>35175</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>184</v>
       </c>
@@ -2653,7 +2663,7 @@
         <v>11025</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>184</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>10185</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>184</v>
       </c>
@@ -2681,7 +2691,7 @@
         <v>8925</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>184</v>
       </c>
@@ -2695,7 +2705,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>184</v>
       </c>
@@ -2709,7 +2719,7 @@
         <v>1212.75</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>184</v>
       </c>
@@ -2723,7 +2733,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -2737,7 +2747,7 @@
         <v>5460</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>184</v>
       </c>
@@ -2751,7 +2761,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>188</v>
       </c>
@@ -2765,7 +2775,7 @@
         <v>1352.5345</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>188</v>
       </c>
@@ -2779,7 +2789,7 @@
         <v>1218.3900000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>188</v>
       </c>
@@ -2793,7 +2803,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>188</v>
       </c>
@@ -2807,7 +2817,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>188</v>
       </c>
@@ -2821,7 +2831,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>188</v>
       </c>
@@ -2835,7 +2845,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>188</v>
       </c>
@@ -2849,7 +2859,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>188</v>
       </c>
@@ -2863,7 +2873,7 @@
         <v>199.5</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -2877,7 +2887,7 @@
         <v>304.5</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>188</v>
       </c>
@@ -2891,7 +2901,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>188</v>
       </c>
@@ -2905,7 +2915,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>188</v>
       </c>
@@ -2919,7 +2929,7 @@
         <v>12600</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>188</v>
       </c>
@@ -2933,7 +2943,7 @@
         <v>30975</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>188</v>
       </c>
@@ -2947,7 +2957,7 @@
         <v>34125</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>188</v>
       </c>
@@ -2961,7 +2971,7 @@
         <v>86100</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>188</v>
       </c>
@@ -2975,7 +2985,7 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>188</v>
       </c>
@@ -2989,7 +2999,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>188</v>
       </c>
@@ -3003,7 +3013,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>188</v>
       </c>
@@ -3017,7 +3027,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>188</v>
       </c>
@@ -3031,7 +3041,7 @@
         <v>51553.5</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -3045,7 +3055,7 @@
         <v>16205.33</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -3059,7 +3069,7 @@
         <v>3675</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>188</v>
       </c>
@@ -3073,7 +3083,7 @@
         <v>4777.5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>188</v>
       </c>
@@ -3087,7 +3097,7 @@
         <v>3675</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>188</v>
       </c>
@@ -3101,7 +3111,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>188</v>
       </c>
@@ -3115,7 +3125,7 @@
         <v>4725</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>188</v>
       </c>
@@ -3129,7 +3139,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>188</v>
       </c>
@@ -3143,7 +3153,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -3157,7 +3167,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>188</v>
       </c>
@@ -3171,7 +3181,7 @@
         <v>3675</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>196</v>
       </c>
@@ -3185,7 +3195,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>196</v>
       </c>
@@ -3199,7 +3209,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>196</v>
       </c>
@@ -3213,7 +3223,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>196</v>
       </c>
@@ -3227,7 +3237,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>196</v>
       </c>
@@ -3241,7 +3251,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>196</v>
       </c>
@@ -3255,7 +3265,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>196</v>
       </c>
@@ -3269,7 +3279,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>196</v>
       </c>
@@ -3283,7 +3293,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>196</v>
       </c>
@@ -3297,7 +3307,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>196</v>
       </c>
@@ -3311,7 +3321,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>196</v>
       </c>
@@ -3325,7 +3335,7 @@
         <v>1522.5</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>196</v>
       </c>
@@ -3339,7 +3349,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>196</v>
       </c>
@@ -3353,7 +3363,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>196</v>
       </c>
@@ -3367,7 +3377,7 @@
         <v>1018.5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>196</v>
       </c>
@@ -3381,7 +3391,7 @@
         <v>787.5</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>196</v>
       </c>
@@ -3395,7 +3405,7 @@
         <v>1732.5</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>196</v>
       </c>
@@ -3409,7 +3419,7 @@
         <v>3097.5</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>196</v>
       </c>
@@ -3423,7 +3433,7 @@
         <v>4725</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>201</v>
       </c>
@@ -3437,7 +3447,7 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>204</v>
       </c>
@@ -3451,7 +3461,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>204</v>
       </c>
@@ -3465,7 +3475,7 @@
         <v>950000</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>204</v>
       </c>
@@ -3479,7 +3489,7 @@
         <v>24500</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>204</v>
       </c>
@@ -3493,7 +3503,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>204</v>
       </c>
@@ -3507,7 +3517,7 @@
         <v>44310</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>204</v>
       </c>
@@ -3521,7 +3531,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>204</v>
       </c>
@@ -3535,7 +3545,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>204</v>
       </c>
@@ -3549,7 +3559,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>204</v>
       </c>
@@ -3563,7 +3573,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>204</v>
       </c>
@@ -3577,7 +3587,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>204</v>
       </c>
@@ -3591,7 +3601,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>204</v>
       </c>
@@ -3605,7 +3615,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>204</v>
       </c>
@@ -3619,7 +3629,7 @@
         <v>335000</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>204</v>
       </c>
@@ -3633,7 +3643,7 @@
         <v>285600</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>204</v>
       </c>
@@ -3647,7 +3657,7 @@
         <v>378000</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>211</v>
       </c>
@@ -3661,7 +3671,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>211</v>
       </c>
@@ -3675,7 +3685,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>211</v>
       </c>
@@ -3689,7 +3699,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>215</v>
       </c>
@@ -3703,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>215</v>
       </c>
@@ -3717,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>218</v>
       </c>
@@ -3731,7 +3741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>218</v>
       </c>
@@ -3745,7 +3755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>218</v>
       </c>
@@ -3759,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>222</v>
       </c>
@@ -3773,7 +3783,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>225</v>
       </c>
@@ -3787,7 +3797,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>225</v>
       </c>
@@ -3801,7 +3811,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>225</v>
       </c>
@@ -3815,7 +3825,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>229</v>
       </c>
@@ -3829,7 +3839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>229</v>
       </c>
@@ -3843,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>229</v>
       </c>
@@ -3857,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>229</v>
       </c>
@@ -3871,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>229</v>
       </c>
@@ -3885,7 +3895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>229</v>
       </c>
@@ -3899,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>229</v>
       </c>
@@ -3913,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>229</v>
       </c>
@@ -3927,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>229</v>
       </c>
@@ -3941,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>229</v>
       </c>
@@ -3955,7 +3965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>229</v>
       </c>
@@ -3969,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>229</v>
       </c>
@@ -3983,1418 +3993,1325 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>243</v>
       </c>
       <c r="B163" t="s">
+        <v>321</v>
+      </c>
+      <c r="C163" t="s">
+        <v>322</v>
+      </c>
+      <c r="D163" s="1">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>243</v>
+      </c>
+      <c r="B164" t="s">
+        <v>282</v>
+      </c>
+      <c r="C164" t="s">
+        <v>298</v>
+      </c>
+      <c r="D164" s="1">
+        <v>71.36</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>243</v>
+      </c>
+      <c r="B165" t="s">
+        <v>283</v>
+      </c>
+      <c r="C165" t="s">
+        <v>284</v>
+      </c>
+      <c r="D165" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>243</v>
+      </c>
+      <c r="B166" t="s">
+        <v>285</v>
+      </c>
+      <c r="C166" t="s">
+        <v>286</v>
+      </c>
+      <c r="D166" s="1">
+        <v>113.99</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>243</v>
+      </c>
+      <c r="B167" t="s">
+        <v>287</v>
+      </c>
+      <c r="C167" t="s">
+        <v>288</v>
+      </c>
+      <c r="D167" s="1">
+        <v>156.04999999999998</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>243</v>
+      </c>
+      <c r="B168" t="s">
+        <v>281</v>
+      </c>
+      <c r="C168" t="s">
+        <v>280</v>
+      </c>
+      <c r="D168" s="1">
+        <v>637.6</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>243</v>
+      </c>
+      <c r="B169" t="s">
+        <v>277</v>
+      </c>
+      <c r="C169" t="s">
+        <v>278</v>
+      </c>
+      <c r="D169" s="1">
+        <v>415.73333333333335</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>243</v>
+      </c>
+      <c r="B170" t="s">
+        <v>279</v>
+      </c>
+      <c r="C170" t="s">
+        <v>280</v>
+      </c>
+      <c r="D170" s="1">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>243</v>
+      </c>
+      <c r="B171" t="s">
+        <v>275</v>
+      </c>
+      <c r="C171" t="s">
+        <v>276</v>
+      </c>
+      <c r="D171" s="1">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>243</v>
+      </c>
+      <c r="B172" t="s">
+        <v>389</v>
+      </c>
+      <c r="C172" t="s">
+        <v>390</v>
+      </c>
+      <c r="D172" s="1">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>243</v>
+      </c>
+      <c r="B173" t="s">
+        <v>268</v>
+      </c>
+      <c r="C173" t="s">
+        <v>269</v>
+      </c>
+      <c r="D173" s="1">
+        <v>5740</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>243</v>
+      </c>
+      <c r="B174" t="s">
+        <v>270</v>
+      </c>
+      <c r="C174" t="s">
+        <v>271</v>
+      </c>
+      <c r="D174" s="1">
+        <v>7010</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>243</v>
+      </c>
+      <c r="B175" t="s">
+        <v>266</v>
+      </c>
+      <c r="C175" t="s">
+        <v>267</v>
+      </c>
+      <c r="D175" s="1">
+        <v>4890</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>243</v>
+      </c>
+      <c r="B176" t="s">
+        <v>264</v>
+      </c>
+      <c r="C176" t="s">
+        <v>265</v>
+      </c>
+      <c r="D176" s="1">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>243</v>
+      </c>
+      <c r="B177" t="s">
         <v>244</v>
       </c>
-      <c r="C163" t="s">
+      <c r="C177" t="s">
         <v>245</v>
       </c>
-      <c r="D163" s="1">
+      <c r="D177" s="1">
         <v>330.8</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
-        <v>243</v>
-      </c>
-      <c r="B164" t="s">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>243</v>
+      </c>
+      <c r="B178" t="s">
+        <v>340</v>
+      </c>
+      <c r="C178" t="s">
+        <v>341</v>
+      </c>
+      <c r="D178" s="1">
+        <v>112.72</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>243</v>
+      </c>
+      <c r="B179" t="s">
+        <v>332</v>
+      </c>
+      <c r="C179" t="s">
+        <v>333</v>
+      </c>
+      <c r="D179" s="1">
+        <v>123.22999999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>243</v>
+      </c>
+      <c r="B180" t="s">
+        <v>391</v>
+      </c>
+      <c r="C180" t="s">
+        <v>392</v>
+      </c>
+      <c r="D180" s="1">
+        <v>13.553333333333333</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>243</v>
+      </c>
+      <c r="B181" t="s">
+        <v>393</v>
+      </c>
+      <c r="C181" t="s">
+        <v>394</v>
+      </c>
+      <c r="D181" s="1">
+        <v>53.010000000000005</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>243</v>
+      </c>
+      <c r="B182" t="s">
+        <v>395</v>
+      </c>
+      <c r="C182" t="s">
+        <v>396</v>
+      </c>
+      <c r="D182" s="1">
+        <v>38.83</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>243</v>
+      </c>
+      <c r="B183" t="s">
         <v>246</v>
       </c>
-      <c r="C164" t="s">
+      <c r="C183" t="s">
         <v>247</v>
       </c>
-      <c r="D164" s="1">
+      <c r="D183" s="1">
         <v>444.5</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A165" t="s">
-        <v>243</v>
-      </c>
-      <c r="B165" t="s">
+      <c r="E183"/>
+    </row>
+    <row r="184" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D184" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>243</v>
+      </c>
+      <c r="B185" t="s">
+        <v>346</v>
+      </c>
+      <c r="C185" t="s">
+        <v>347</v>
+      </c>
+      <c r="D185" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>243</v>
+      </c>
+      <c r="B186" t="s">
+        <v>348</v>
+      </c>
+      <c r="C186" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D186" s="1">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>243</v>
+      </c>
+      <c r="B187" t="s">
+        <v>350</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D187" s="1">
+        <v>24.024999999999999</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>243</v>
+      </c>
+      <c r="B188" t="s">
+        <v>352</v>
+      </c>
+      <c r="C188" t="s">
+        <v>353</v>
+      </c>
+      <c r="D188" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>243</v>
+      </c>
+      <c r="B189" t="s">
+        <v>364</v>
+      </c>
+      <c r="C189" t="s">
+        <v>365</v>
+      </c>
+      <c r="D189" s="1">
+        <v>1735.335</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>243</v>
+      </c>
+      <c r="B190" t="s">
+        <v>366</v>
+      </c>
+      <c r="C190" t="s">
+        <v>365</v>
+      </c>
+      <c r="D190" s="1">
+        <v>166.435</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>243</v>
+      </c>
+      <c r="B191" t="s">
+        <v>397</v>
+      </c>
+      <c r="C191" t="s">
+        <v>398</v>
+      </c>
+      <c r="D191" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>243</v>
+      </c>
+      <c r="B192" t="s">
+        <v>399</v>
+      </c>
+      <c r="C192" t="s">
+        <v>400</v>
+      </c>
+      <c r="D192" s="1">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E192"/>
+    </row>
+    <row r="193" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>243</v>
+      </c>
+      <c r="B193" t="s">
+        <v>417</v>
+      </c>
+      <c r="C193" t="s">
+        <v>418</v>
+      </c>
+      <c r="D193" s="1">
+        <v>725</v>
+      </c>
+      <c r="E193"/>
+    </row>
+    <row r="194" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>243</v>
+      </c>
+      <c r="B194" t="s">
+        <v>401</v>
+      </c>
+      <c r="C194" t="s">
+        <v>402</v>
+      </c>
+      <c r="D194" s="1">
+        <v>10.25</v>
+      </c>
+      <c r="E194"/>
+    </row>
+    <row r="195" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>243</v>
+      </c>
+      <c r="B195" t="s">
+        <v>290</v>
+      </c>
+      <c r="C195" t="s">
+        <v>291</v>
+      </c>
+      <c r="D195" s="1">
+        <v>76.5</v>
+      </c>
+      <c r="E195"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>243</v>
+      </c>
+      <c r="B196" t="s">
+        <v>292</v>
+      </c>
+      <c r="C196" t="s">
+        <v>293</v>
+      </c>
+      <c r="D196" s="1">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D197" s="5">
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D198" s="5">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>243</v>
+      </c>
+      <c r="B199" t="s">
+        <v>323</v>
+      </c>
+      <c r="C199" t="s">
+        <v>324</v>
+      </c>
+      <c r="D199" s="1">
+        <v>194.23000000000002</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>243</v>
+      </c>
+      <c r="B200" t="s">
         <v>248</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C200" t="s">
         <v>249</v>
       </c>
-      <c r="D165" s="1">
+      <c r="D200" s="1">
         <v>621.14499999999998</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A166" t="s">
-        <v>243</v>
-      </c>
-      <c r="B166" t="s">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>243</v>
+      </c>
+      <c r="B201" t="s">
+        <v>403</v>
+      </c>
+      <c r="C201" t="s">
+        <v>404</v>
+      </c>
+      <c r="D201" s="1">
+        <v>8.65</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>243</v>
+      </c>
+      <c r="B202" t="s">
         <v>250</v>
       </c>
-      <c r="C166" t="s">
+      <c r="C202" t="s">
         <v>251</v>
       </c>
-      <c r="D166" s="1">
+      <c r="D202" s="1">
         <v>707.85</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A167" t="s">
-        <v>243</v>
-      </c>
-      <c r="B167" t="s">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>243</v>
+      </c>
+      <c r="B203" t="s">
         <v>252</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C203" t="s">
         <v>253</v>
       </c>
-      <c r="D167" s="1">
+      <c r="D203" s="1">
         <v>857.93000000000006</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A168" t="s">
-        <v>243</v>
-      </c>
-      <c r="B168" t="s">
-        <v>254</v>
-      </c>
-      <c r="C168" t="s">
-        <v>255</v>
-      </c>
-      <c r="D168" s="1">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A169" t="s">
-        <v>243</v>
-      </c>
-      <c r="B169" t="s">
-        <v>256</v>
-      </c>
-      <c r="C169" t="s">
-        <v>257</v>
-      </c>
-      <c r="D169" s="1">
-        <v>1089.6799999999998</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
-        <v>243</v>
-      </c>
-      <c r="B170" t="s">
-        <v>258</v>
-      </c>
-      <c r="C170" t="s">
-        <v>259</v>
-      </c>
-      <c r="D170" s="1">
-        <v>801.10500000000002</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A171" t="s">
-        <v>243</v>
-      </c>
-      <c r="B171" t="s">
-        <v>260</v>
-      </c>
-      <c r="C171" t="s">
-        <v>261</v>
-      </c>
-      <c r="D171" s="1">
-        <v>335.22</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A172" t="s">
-        <v>243</v>
-      </c>
-      <c r="B172" t="s">
-        <v>262</v>
-      </c>
-      <c r="C172" t="s">
-        <v>263</v>
-      </c>
-      <c r="D172" s="1">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A173" t="s">
-        <v>243</v>
-      </c>
-      <c r="B173" t="s">
-        <v>264</v>
-      </c>
-      <c r="C173" t="s">
-        <v>265</v>
-      </c>
-      <c r="D173" s="1">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A174" t="s">
-        <v>243</v>
-      </c>
-      <c r="B174" t="s">
-        <v>266</v>
-      </c>
-      <c r="C174" t="s">
-        <v>267</v>
-      </c>
-      <c r="D174" s="1">
-        <v>4890</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A175" t="s">
-        <v>243</v>
-      </c>
-      <c r="B175" t="s">
-        <v>268</v>
-      </c>
-      <c r="C175" t="s">
-        <v>269</v>
-      </c>
-      <c r="D175" s="1">
-        <v>5740</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A176" t="s">
-        <v>243</v>
-      </c>
-      <c r="B176" t="s">
-        <v>270</v>
-      </c>
-      <c r="C176" t="s">
-        <v>271</v>
-      </c>
-      <c r="D176" s="1">
-        <v>7010</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A177" t="s">
-        <v>243</v>
-      </c>
-      <c r="B177" t="s">
-        <v>272</v>
-      </c>
-      <c r="C177" t="s">
-        <v>273</v>
-      </c>
-      <c r="D177" s="1">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A178" t="s">
-        <v>243</v>
-      </c>
-      <c r="B178" t="s">
-        <v>274</v>
-      </c>
-      <c r="C178" t="s">
-        <v>273</v>
-      </c>
-      <c r="D178" s="1">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A179" t="s">
-        <v>243</v>
-      </c>
-      <c r="B179" t="s">
-        <v>275</v>
-      </c>
-      <c r="C179" t="s">
-        <v>276</v>
-      </c>
-      <c r="D179" s="1">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A180" t="s">
-        <v>243</v>
-      </c>
-      <c r="B180" t="s">
-        <v>277</v>
-      </c>
-      <c r="C180" t="s">
-        <v>278</v>
-      </c>
-      <c r="D180" s="1">
-        <v>415.73333333333335</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A181" t="s">
-        <v>243</v>
-      </c>
-      <c r="B181" t="s">
-        <v>279</v>
-      </c>
-      <c r="C181" t="s">
-        <v>280</v>
-      </c>
-      <c r="D181" s="1">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A182" t="s">
-        <v>243</v>
-      </c>
-      <c r="B182" t="s">
-        <v>281</v>
-      </c>
-      <c r="C182" t="s">
-        <v>280</v>
-      </c>
-      <c r="D182" s="1">
-        <v>637.6</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A183" t="s">
-        <v>243</v>
-      </c>
-      <c r="B183" t="s">
-        <v>282</v>
-      </c>
-      <c r="C183" t="s">
-        <v>283</v>
-      </c>
-      <c r="D183" s="1">
-        <v>71.36</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A184" t="s">
-        <v>243</v>
-      </c>
-      <c r="B184" t="s">
-        <v>284</v>
-      </c>
-      <c r="C184" t="s">
-        <v>285</v>
-      </c>
-      <c r="D184" s="1">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A185" t="s">
-        <v>243</v>
-      </c>
-      <c r="B185" t="s">
-        <v>286</v>
-      </c>
-      <c r="C185" t="s">
-        <v>287</v>
-      </c>
-      <c r="D185" s="1">
-        <v>113.99</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A186" t="s">
-        <v>243</v>
-      </c>
-      <c r="B186" t="s">
-        <v>288</v>
-      </c>
-      <c r="C186" t="s">
-        <v>289</v>
-      </c>
-      <c r="D186" s="1">
-        <v>156.04999999999998</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A187" t="s">
-        <v>243</v>
-      </c>
-      <c r="B187" t="s">
-        <v>290</v>
-      </c>
-      <c r="C187" t="s">
-        <v>291</v>
-      </c>
-      <c r="D187" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
-        <v>243</v>
-      </c>
-      <c r="B188" t="s">
-        <v>292</v>
-      </c>
-      <c r="C188" t="s">
-        <v>293</v>
-      </c>
-      <c r="D188" s="1">
-        <v>76.5</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
-        <v>243</v>
-      </c>
-      <c r="B189" t="s">
-        <v>294</v>
-      </c>
-      <c r="C189" t="s">
-        <v>295</v>
-      </c>
-      <c r="D189" s="1">
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
-        <v>243</v>
-      </c>
-      <c r="B190" t="s">
-        <v>296</v>
-      </c>
-      <c r="C190" t="s">
-        <v>297</v>
-      </c>
-      <c r="D190" s="1">
-        <v>71.5</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>243</v>
-      </c>
-      <c r="B191" t="s">
-        <v>298</v>
-      </c>
-      <c r="C191" t="s">
-        <v>299</v>
-      </c>
-      <c r="D191" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>243</v>
-      </c>
-      <c r="B192" t="s">
-        <v>300</v>
-      </c>
-      <c r="C192" t="s">
-        <v>301</v>
-      </c>
-      <c r="D192" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
-        <v>243</v>
-      </c>
-      <c r="B193" t="s">
-        <v>282</v>
-      </c>
-      <c r="C193" t="s">
-        <v>302</v>
-      </c>
-      <c r="D193" s="1">
-        <v>71.36</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
-        <v>243</v>
-      </c>
-      <c r="B194" t="s">
-        <v>284</v>
-      </c>
-      <c r="C194" t="s">
-        <v>285</v>
-      </c>
-      <c r="D194" s="1">
-        <v>5.3</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
-        <v>243</v>
-      </c>
-      <c r="B195" t="s">
-        <v>286</v>
-      </c>
-      <c r="C195" t="s">
-        <v>303</v>
-      </c>
-      <c r="D195" s="1">
-        <v>113.99</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>243</v>
-      </c>
-      <c r="B196" t="s">
-        <v>288</v>
-      </c>
-      <c r="C196" t="s">
-        <v>304</v>
-      </c>
-      <c r="D196" s="1">
-        <v>156.04999999999998</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>243</v>
-      </c>
-      <c r="B197" t="s">
-        <v>290</v>
-      </c>
-      <c r="C197" t="s">
-        <v>305</v>
-      </c>
-      <c r="D197" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>243</v>
-      </c>
-      <c r="B198" t="s">
-        <v>306</v>
-      </c>
-      <c r="C198" t="s">
-        <v>307</v>
-      </c>
-      <c r="D198" s="1">
-        <v>82.5</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
-        <v>243</v>
-      </c>
-      <c r="B199" t="s">
-        <v>308</v>
-      </c>
-      <c r="C199" t="s">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>243</v>
+      </c>
+      <c r="B204" t="s">
         <v>309</v>
       </c>
-      <c r="D199" s="1">
-        <v>74.5</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
-        <v>243</v>
-      </c>
-      <c r="B200" t="s">
-        <v>296</v>
-      </c>
-      <c r="C200" t="s">
+      <c r="C204" t="s">
         <v>310</v>
-      </c>
-      <c r="D200" s="1">
-        <v>71.5</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
-        <v>243</v>
-      </c>
-      <c r="B201" t="s">
-        <v>311</v>
-      </c>
-      <c r="C201" t="s">
-        <v>312</v>
-      </c>
-      <c r="D201" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
-        <v>243</v>
-      </c>
-      <c r="B202" t="s">
-        <v>300</v>
-      </c>
-      <c r="C202" t="s">
-        <v>313</v>
-      </c>
-      <c r="D202" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A203" t="s">
-        <v>243</v>
-      </c>
-      <c r="B203" t="s">
-        <v>314</v>
-      </c>
-      <c r="C203" t="s">
-        <v>315</v>
-      </c>
-      <c r="D203" s="1">
-        <v>1059.0349999999999</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A204" t="s">
-        <v>243</v>
-      </c>
-      <c r="B204" t="s">
-        <v>316</v>
-      </c>
-      <c r="C204" t="s">
-        <v>317</v>
       </c>
       <c r="D204" s="1">
         <v>1765</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>243</v>
       </c>
       <c r="B205" t="s">
-        <v>90</v>
+        <v>307</v>
       </c>
       <c r="C205" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="D205" s="1">
-        <v>91.465000000000003</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1059.0349999999999</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>243</v>
       </c>
       <c r="B206" t="s">
-        <v>319</v>
+        <v>254</v>
       </c>
       <c r="C206" t="s">
-        <v>320</v>
+        <v>255</v>
       </c>
       <c r="D206" s="1">
-        <v>33.244999999999997</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>243</v>
       </c>
       <c r="B207" t="s">
-        <v>321</v>
+        <v>405</v>
       </c>
       <c r="C207" t="s">
-        <v>322</v>
+        <v>406</v>
       </c>
       <c r="D207" s="1">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+        <v>90.61</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>243</v>
       </c>
       <c r="B208" t="s">
-        <v>323</v>
+        <v>407</v>
       </c>
       <c r="C208" t="s">
-        <v>324</v>
+        <v>408</v>
       </c>
       <c r="D208" s="1">
-        <v>187.5</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+        <v>13.84</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>243</v>
       </c>
       <c r="B209" t="s">
+        <v>409</v>
+      </c>
+      <c r="C209" t="s">
+        <v>410</v>
+      </c>
+      <c r="D209" s="1">
+        <v>28.93</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D210" s="5">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>243</v>
+      </c>
+      <c r="B211" t="s">
+        <v>304</v>
+      </c>
+      <c r="C211" t="s">
+        <v>305</v>
+      </c>
+      <c r="D211" s="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>243</v>
+      </c>
+      <c r="B212" t="s">
+        <v>256</v>
+      </c>
+      <c r="C212" t="s">
+        <v>257</v>
+      </c>
+      <c r="D212" s="1">
+        <v>1089.6799999999998</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>243</v>
+      </c>
+      <c r="B213" t="s">
+        <v>411</v>
+      </c>
+      <c r="C213" t="s">
+        <v>412</v>
+      </c>
+      <c r="D213" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>243</v>
+      </c>
+      <c r="B214" t="s">
+        <v>413</v>
+      </c>
+      <c r="C214" t="s">
+        <v>414</v>
+      </c>
+      <c r="D214" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>243</v>
+      </c>
+      <c r="B215" t="s">
+        <v>415</v>
+      </c>
+      <c r="C215" t="s">
+        <v>416</v>
+      </c>
+      <c r="D215" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>243</v>
+      </c>
+      <c r="B216" t="s">
         <v>325</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C216" t="s">
         <v>326</v>
       </c>
-      <c r="D209" s="1">
-        <v>390.73500000000001</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A210" t="s">
-        <v>243</v>
-      </c>
-      <c r="B210" t="s">
-        <v>327</v>
-      </c>
-      <c r="C210" t="s">
-        <v>326</v>
-      </c>
-      <c r="D210" s="1">
-        <v>1094.6799999999998</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
-        <v>243</v>
-      </c>
-      <c r="B211" t="s">
-        <v>328</v>
-      </c>
-      <c r="C211" t="s">
-        <v>329</v>
-      </c>
-      <c r="D211" s="1">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A212" t="s">
-        <v>243</v>
-      </c>
-      <c r="B212" t="s">
-        <v>330</v>
-      </c>
-      <c r="C212" t="s">
-        <v>331</v>
-      </c>
-      <c r="D212" s="1">
-        <v>194.23000000000002</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A213" t="s">
-        <v>243</v>
-      </c>
-      <c r="B213" t="s">
-        <v>332</v>
-      </c>
-      <c r="C213" t="s">
-        <v>333</v>
-      </c>
-      <c r="D213" s="1">
+      <c r="D216" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A214" t="s">
-        <v>243</v>
-      </c>
-      <c r="B214" t="s">
-        <v>334</v>
-      </c>
-      <c r="C214" t="s">
-        <v>335</v>
-      </c>
-      <c r="D214" s="1">
-        <v>131.92000000000002</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A215" t="s">
-        <v>243</v>
-      </c>
-      <c r="B215" t="s">
-        <v>336</v>
-      </c>
-      <c r="C215" t="s">
-        <v>337</v>
-      </c>
-      <c r="D215" s="1">
-        <v>33.42</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
-        <v>243</v>
-      </c>
-      <c r="B216" t="s">
-        <v>136</v>
-      </c>
-      <c r="C216" t="s">
-        <v>338</v>
-      </c>
-      <c r="D216" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>243</v>
       </c>
       <c r="B217" t="s">
-        <v>339</v>
+        <v>295</v>
       </c>
       <c r="C217" t="s">
-        <v>340</v>
+        <v>296</v>
       </c>
       <c r="D217" s="1">
-        <v>123.22999999999999</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>243</v>
       </c>
       <c r="B218" t="s">
-        <v>341</v>
+        <v>86</v>
       </c>
       <c r="C218" t="s">
-        <v>342</v>
+        <v>354</v>
       </c>
       <c r="D218" s="1">
-        <v>126.25</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>243</v>
       </c>
       <c r="B219" t="s">
-        <v>343</v>
+        <v>355</v>
       </c>
       <c r="C219" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
       <c r="D219" s="1">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+        <v>89.5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>243</v>
       </c>
       <c r="B220" t="s">
-        <v>158</v>
+        <v>357</v>
       </c>
       <c r="C220" t="s">
-        <v>345</v>
+        <v>357</v>
       </c>
       <c r="D220" s="1">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>243</v>
       </c>
       <c r="B221" t="s">
-        <v>137</v>
+        <v>358</v>
       </c>
       <c r="C221" t="s">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="D221" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>243</v>
       </c>
       <c r="B222" t="s">
-        <v>347</v>
+        <v>360</v>
       </c>
       <c r="C222" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="D222" s="1">
-        <v>112.72</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.35">
+        <v>250.965</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>243</v>
       </c>
       <c r="B223" t="s">
-        <v>349</v>
+        <v>90</v>
       </c>
       <c r="C223" t="s">
+        <v>311</v>
+      </c>
+      <c r="D223" s="1">
+        <v>91.465000000000003</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>243</v>
+      </c>
+      <c r="B224" t="s">
+        <v>367</v>
+      </c>
+      <c r="C224" t="s">
+        <v>368</v>
+      </c>
+      <c r="D224" s="1">
+        <v>2350</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>243</v>
+      </c>
+      <c r="B225" t="s">
+        <v>369</v>
+      </c>
+      <c r="C225" t="s">
+        <v>370</v>
+      </c>
+      <c r="D225" s="1">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>243</v>
+      </c>
+      <c r="B226" t="s">
+        <v>327</v>
+      </c>
+      <c r="C226" t="s">
+        <v>328</v>
+      </c>
+      <c r="D226" s="1">
+        <v>131.92000000000002</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>243</v>
+      </c>
+      <c r="B227" t="s">
+        <v>371</v>
+      </c>
+      <c r="C227" t="s">
+        <v>372</v>
+      </c>
+      <c r="D227" s="1">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>243</v>
+      </c>
+      <c r="B228" t="s">
+        <v>373</v>
+      </c>
+      <c r="C228" t="s">
+        <v>374</v>
+      </c>
+      <c r="D228" s="1">
         <v>350</v>
       </c>
-      <c r="D223" s="1">
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>243</v>
+      </c>
+      <c r="B229" t="s">
+        <v>362</v>
+      </c>
+      <c r="C229" t="s">
+        <v>363</v>
+      </c>
+      <c r="D229" s="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>243</v>
+      </c>
+      <c r="B230" t="s">
+        <v>312</v>
+      </c>
+      <c r="C230" t="s">
+        <v>313</v>
+      </c>
+      <c r="D230" s="1">
+        <v>33.244999999999997</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>243</v>
+      </c>
+      <c r="B231" t="s">
+        <v>297</v>
+      </c>
+      <c r="C231" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D231" s="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>243</v>
+      </c>
+      <c r="B232" t="s">
+        <v>329</v>
+      </c>
+      <c r="C232" t="s">
+        <v>330</v>
+      </c>
+      <c r="D232" s="1">
+        <v>33.42</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>243</v>
+      </c>
+      <c r="B233" t="s">
+        <v>314</v>
+      </c>
+      <c r="C233" t="s">
+        <v>315</v>
+      </c>
+      <c r="D233" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>243</v>
+      </c>
+      <c r="B234" t="s">
+        <v>316</v>
+      </c>
+      <c r="C234" t="s">
+        <v>317</v>
+      </c>
+      <c r="D234" s="1">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>243</v>
+      </c>
+      <c r="B235" t="s">
+        <v>258</v>
+      </c>
+      <c r="C235" t="s">
+        <v>259</v>
+      </c>
+      <c r="D235" s="1">
+        <v>801.10500000000002</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>243</v>
+      </c>
+      <c r="B236" t="s">
+        <v>272</v>
+      </c>
+      <c r="C236" t="s">
+        <v>273</v>
+      </c>
+      <c r="D236" s="1">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>243</v>
+      </c>
+      <c r="B237" t="s">
+        <v>274</v>
+      </c>
+      <c r="C237" t="s">
+        <v>273</v>
+      </c>
+      <c r="D237" s="1">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>243</v>
+      </c>
+      <c r="B238" t="s">
+        <v>136</v>
+      </c>
+      <c r="C238" t="s">
+        <v>331</v>
+      </c>
+      <c r="D238" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>243</v>
+      </c>
+      <c r="B239" t="s">
+        <v>260</v>
+      </c>
+      <c r="C239" t="s">
+        <v>261</v>
+      </c>
+      <c r="D239" s="1">
+        <v>335.22</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>243</v>
+      </c>
+      <c r="B240" t="s">
+        <v>262</v>
+      </c>
+      <c r="C240" t="s">
+        <v>263</v>
+      </c>
+      <c r="D240" s="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>243</v>
+      </c>
+      <c r="B241" t="s">
+        <v>318</v>
+      </c>
+      <c r="C241" t="s">
+        <v>319</v>
+      </c>
+      <c r="D241" s="1">
+        <v>390.73500000000001</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>243</v>
+      </c>
+      <c r="B242" t="s">
+        <v>320</v>
+      </c>
+      <c r="C242" t="s">
+        <v>319</v>
+      </c>
+      <c r="D242" s="1">
+        <v>1094.6799999999998</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>243</v>
+      </c>
+      <c r="B243" t="s">
+        <v>336</v>
+      </c>
+      <c r="C243" t="s">
+        <v>337</v>
+      </c>
+      <c r="D243" s="1">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>342</v>
+      </c>
+      <c r="C244" t="s">
+        <v>343</v>
+      </c>
+      <c r="D244" s="1">
         <v>31.25</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A224" t="s">
-        <v>243</v>
-      </c>
-      <c r="B224" t="s">
-        <v>351</v>
-      </c>
-      <c r="C224" t="s">
-        <v>352</v>
-      </c>
-      <c r="D224" s="1">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>243</v>
+      </c>
+      <c r="B245" t="s">
+        <v>344</v>
+      </c>
+      <c r="C245" t="s">
+        <v>345</v>
+      </c>
+      <c r="D245" s="1">
         <v>37.5</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A225" t="s">
-        <v>243</v>
-      </c>
-      <c r="B225" t="s">
-        <v>353</v>
-      </c>
-      <c r="C225" t="s">
-        <v>354</v>
-      </c>
-      <c r="D225" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A226" t="s">
-        <v>243</v>
-      </c>
-      <c r="B226" t="s">
-        <v>355</v>
-      </c>
-      <c r="C226" t="s">
-        <v>356</v>
-      </c>
-      <c r="D226" s="1">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A227" t="s">
-        <v>243</v>
-      </c>
-      <c r="B227" t="s">
-        <v>357</v>
-      </c>
-      <c r="C227" t="s">
-        <v>358</v>
-      </c>
-      <c r="D227" s="1">
-        <v>24.024999999999999</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A228" t="s">
-        <v>243</v>
-      </c>
-      <c r="B228" t="s">
-        <v>359</v>
-      </c>
-      <c r="C228" t="s">
-        <v>360</v>
-      </c>
-      <c r="D228" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A229" t="s">
-        <v>243</v>
-      </c>
-      <c r="B229" t="s">
-        <v>86</v>
-      </c>
-      <c r="C229" t="s">
-        <v>361</v>
-      </c>
-      <c r="D229" s="1">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
-        <v>243</v>
-      </c>
-      <c r="B230" t="s">
-        <v>362</v>
-      </c>
-      <c r="C230" t="s">
-        <v>363</v>
-      </c>
-      <c r="D230" s="1">
-        <v>89.5</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A231" t="s">
-        <v>243</v>
-      </c>
-      <c r="B231" t="s">
-        <v>364</v>
-      </c>
-      <c r="C231" t="s">
-        <v>364</v>
-      </c>
-      <c r="D231" s="1">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A232" t="s">
-        <v>243</v>
-      </c>
-      <c r="B232" t="s">
-        <v>365</v>
-      </c>
-      <c r="C232" t="s">
-        <v>366</v>
-      </c>
-      <c r="D232" s="1">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>243</v>
+      </c>
+      <c r="B246" t="s">
+        <v>334</v>
+      </c>
+      <c r="C246" t="s">
+        <v>335</v>
+      </c>
+      <c r="D246" s="1">
+        <v>126.25</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>243</v>
+      </c>
+      <c r="B247" t="s">
+        <v>158</v>
+      </c>
+      <c r="C247" t="s">
+        <v>338</v>
+      </c>
+      <c r="D247" s="1">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>243</v>
+      </c>
+      <c r="B248" t="s">
+        <v>375</v>
+      </c>
+      <c r="C248" t="s">
+        <v>376</v>
+      </c>
+      <c r="D248" s="1">
+        <v>1633.41</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>243</v>
+      </c>
+      <c r="B249" t="s">
+        <v>377</v>
+      </c>
+      <c r="C249" t="s">
+        <v>376</v>
+      </c>
+      <c r="D249" s="1">
+        <v>163.34</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>243</v>
+      </c>
+      <c r="B250" t="s">
+        <v>380</v>
+      </c>
+      <c r="C250" t="s">
+        <v>379</v>
+      </c>
+      <c r="D250" s="1">
+        <v>178.34</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>243</v>
+      </c>
+      <c r="B251" t="s">
+        <v>378</v>
+      </c>
+      <c r="C251" t="s">
+        <v>379</v>
+      </c>
+      <c r="D251" s="1">
+        <v>1783.41</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>243</v>
+      </c>
+      <c r="B252" t="s">
+        <v>381</v>
+      </c>
+      <c r="C252" t="s">
+        <v>382</v>
+      </c>
+      <c r="D252" s="1">
+        <v>938.32500000000005</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>243</v>
+      </c>
+      <c r="B253" t="s">
+        <v>383</v>
+      </c>
+      <c r="C253" t="s">
+        <v>384</v>
+      </c>
+      <c r="D253" s="1">
+        <v>97.986666666666665</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>243</v>
+      </c>
+      <c r="B254" t="s">
+        <v>385</v>
+      </c>
+      <c r="C254" t="s">
+        <v>386</v>
+      </c>
+      <c r="D254" s="1">
+        <v>678.56500000000005</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>243</v>
+      </c>
+      <c r="B255" t="s">
+        <v>387</v>
+      </c>
+      <c r="C255" t="s">
+        <v>388</v>
+      </c>
+      <c r="D255" s="1">
+        <v>67.85499999999999</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>243</v>
+      </c>
+      <c r="B256" t="s">
+        <v>137</v>
+      </c>
+      <c r="C256" t="s">
+        <v>339</v>
+      </c>
+      <c r="D256" s="1">
         <v>150</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
-        <v>243</v>
-      </c>
-      <c r="B233" t="s">
-        <v>367</v>
-      </c>
-      <c r="C233" t="s">
-        <v>368</v>
-      </c>
-      <c r="D233" s="1">
-        <v>250.965</v>
-      </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A234" t="s">
-        <v>243</v>
-      </c>
-      <c r="B234" t="s">
-        <v>369</v>
-      </c>
-      <c r="C234" t="s">
-        <v>370</v>
-      </c>
-      <c r="D234" s="1">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A235" t="s">
-        <v>243</v>
-      </c>
-      <c r="B235" t="s">
-        <v>371</v>
-      </c>
-      <c r="C235" t="s">
-        <v>372</v>
-      </c>
-      <c r="D235" s="1">
-        <v>1735.335</v>
-      </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A236" t="s">
-        <v>243</v>
-      </c>
-      <c r="B236" t="s">
-        <v>373</v>
-      </c>
-      <c r="C236" t="s">
-        <v>372</v>
-      </c>
-      <c r="D236" s="1">
-        <v>166.435</v>
-      </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A237" t="s">
-        <v>243</v>
-      </c>
-      <c r="B237" t="s">
-        <v>374</v>
-      </c>
-      <c r="C237" t="s">
-        <v>375</v>
-      </c>
-      <c r="D237" s="1">
-        <v>2350</v>
-      </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A238" t="s">
-        <v>243</v>
-      </c>
-      <c r="B238" t="s">
-        <v>376</v>
-      </c>
-      <c r="C238" t="s">
-        <v>377</v>
-      </c>
-      <c r="D238" s="1">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
-        <v>243</v>
-      </c>
-      <c r="B239" t="s">
-        <v>378</v>
-      </c>
-      <c r="C239" t="s">
-        <v>379</v>
-      </c>
-      <c r="D239" s="1">
-        <v>3250</v>
-      </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A240" t="s">
-        <v>243</v>
-      </c>
-      <c r="B240" t="s">
-        <v>380</v>
-      </c>
-      <c r="C240" t="s">
-        <v>381</v>
-      </c>
-      <c r="D240" s="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
-        <v>243</v>
-      </c>
-      <c r="B241" t="s">
-        <v>382</v>
-      </c>
-      <c r="C241" t="s">
-        <v>383</v>
-      </c>
-      <c r="D241" s="1">
-        <v>1633.41</v>
-      </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A242" t="s">
-        <v>243</v>
-      </c>
-      <c r="B242" t="s">
-        <v>384</v>
-      </c>
-      <c r="C242" t="s">
-        <v>383</v>
-      </c>
-      <c r="D242" s="1">
-        <v>163.34</v>
-      </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A243" t="s">
-        <v>243</v>
-      </c>
-      <c r="B243" t="s">
-        <v>385</v>
-      </c>
-      <c r="C243" t="s">
-        <v>386</v>
-      </c>
-      <c r="D243" s="1">
-        <v>1783.41</v>
-      </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A244" t="s">
-        <v>243</v>
-      </c>
-      <c r="B244" t="s">
-        <v>387</v>
-      </c>
-      <c r="C244" t="s">
-        <v>386</v>
-      </c>
-      <c r="D244" s="1">
-        <v>178.34</v>
-      </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A245" t="s">
-        <v>243</v>
-      </c>
-      <c r="B245" t="s">
-        <v>388</v>
-      </c>
-      <c r="C245" t="s">
-        <v>389</v>
-      </c>
-      <c r="D245" s="1">
-        <v>938.32500000000005</v>
-      </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A246" t="s">
-        <v>243</v>
-      </c>
-      <c r="B246" t="s">
-        <v>390</v>
-      </c>
-      <c r="C246" t="s">
-        <v>391</v>
-      </c>
-      <c r="D246" s="1">
-        <v>97.986666666666665</v>
-      </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
-        <v>243</v>
-      </c>
-      <c r="B247" t="s">
-        <v>392</v>
-      </c>
-      <c r="C247" t="s">
-        <v>393</v>
-      </c>
-      <c r="D247" s="1">
-        <v>678.56500000000005</v>
-      </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A248" t="s">
-        <v>243</v>
-      </c>
-      <c r="B248" t="s">
-        <v>394</v>
-      </c>
-      <c r="C248" t="s">
-        <v>395</v>
-      </c>
-      <c r="D248" s="1">
-        <v>67.85499999999999</v>
-      </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A249" t="s">
-        <v>243</v>
-      </c>
-      <c r="B249" t="s">
-        <v>396</v>
-      </c>
-      <c r="C249" t="s">
-        <v>397</v>
-      </c>
-      <c r="D249" s="1">
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>243</v>
-      </c>
-      <c r="B250" t="s">
-        <v>398</v>
-      </c>
-      <c r="C250" t="s">
-        <v>399</v>
-      </c>
-      <c r="D250" s="1">
-        <v>13.553333333333333</v>
-      </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>243</v>
-      </c>
-      <c r="B251" t="s">
-        <v>400</v>
-      </c>
-      <c r="C251" t="s">
-        <v>401</v>
-      </c>
-      <c r="D251" s="1">
-        <v>53.010000000000005</v>
-      </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
-        <v>243</v>
-      </c>
-      <c r="B252" t="s">
-        <v>402</v>
-      </c>
-      <c r="C252" t="s">
-        <v>403</v>
-      </c>
-      <c r="D252" s="1">
-        <v>38.83</v>
-      </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
-        <v>243</v>
-      </c>
-      <c r="B253" t="s">
-        <v>404</v>
-      </c>
-      <c r="C253" t="s">
-        <v>405</v>
-      </c>
-      <c r="D253" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
-        <v>243</v>
-      </c>
-      <c r="B254" t="s">
-        <v>406</v>
-      </c>
-      <c r="C254" t="s">
-        <v>407</v>
-      </c>
-      <c r="D254" s="1">
-        <v>9.5500000000000007</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
-        <v>243</v>
-      </c>
-      <c r="B255" t="s">
-        <v>408</v>
-      </c>
-      <c r="C255" t="s">
-        <v>409</v>
-      </c>
-      <c r="D255" s="1">
-        <v>10.25</v>
-      </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>243</v>
-      </c>
-      <c r="B256" t="s">
-        <v>410</v>
-      </c>
-      <c r="C256" t="s">
-        <v>411</v>
-      </c>
-      <c r="D256" s="1">
-        <v>8.65</v>
-      </c>
-    </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>243</v>
-      </c>
-      <c r="B257" t="s">
-        <v>412</v>
-      </c>
-      <c r="C257" t="s">
-        <v>413</v>
-      </c>
-      <c r="D257" s="1">
-        <v>90.61</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
-        <v>243</v>
-      </c>
-      <c r="B258" t="s">
-        <v>414</v>
-      </c>
-      <c r="C258" t="s">
-        <v>415</v>
-      </c>
-      <c r="D258" s="1">
-        <v>13.84</v>
-      </c>
-    </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>243</v>
-      </c>
-      <c r="B259" t="s">
-        <v>416</v>
-      </c>
-      <c r="C259" t="s">
-        <v>417</v>
-      </c>
-      <c r="D259" s="1">
-        <v>28.93</v>
-      </c>
-    </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A260" t="s">
-        <v>243</v>
-      </c>
-      <c r="B260" t="s">
-        <v>418</v>
-      </c>
-      <c r="C260" t="s">
-        <v>419</v>
-      </c>
-      <c r="D260" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A261" t="s">
-        <v>243</v>
-      </c>
-      <c r="B261" t="s">
-        <v>420</v>
-      </c>
-      <c r="C261" t="s">
-        <v>421</v>
-      </c>
-      <c r="D261" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A262" t="s">
-        <v>243</v>
-      </c>
-      <c r="B262" t="s">
-        <v>422</v>
-      </c>
-      <c r="C262" t="s">
-        <v>423</v>
-      </c>
-      <c r="D262" s="1">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A263" t="s">
-        <v>243</v>
-      </c>
-      <c r="B263" t="s">
-        <v>424</v>
-      </c>
-      <c r="C263" t="s">
-        <v>425</v>
-      </c>
-      <c r="D263" s="1">
-        <v>725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>